<commit_message>
Version 09/01 - more objects added
</commit_message>
<xml_diff>
--- a/myexcelproject/OR/ObjectRepository.xlsx
+++ b/myexcelproject/OR/ObjectRepository.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishna.teja.taduri\git\ExcelTestFramework\myexcelproject\OR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{28CBD95D-BC60-41BD-9690-8099CFC2CFA6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5DD8761F-D24A-4DF4-92F8-F4705EB981B8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="80" windowWidth="20060" windowHeight="7940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="80" windowWidth="20060" windowHeight="7940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Object</t>
   </si>
@@ -49,6 +49,21 @@
   </si>
   <si>
     <t>btnHome</t>
+  </si>
+  <si>
+    <t>ddlSelectName</t>
+  </si>
+  <si>
+    <t>//select[@id='userSelect']</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>btnLogin</t>
+  </si>
+  <si>
+    <t>//button[@type='submit']</t>
   </si>
 </sst>
 </file>
@@ -434,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -488,10 +503,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,6 +536,34 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Version_13_01 Added code to handle functions
</commit_message>
<xml_diff>
--- a/myexcelproject/OR/ObjectRepository.xlsx
+++ b/myexcelproject/OR/ObjectRepository.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishna.teja.taduri\git\ExcelTestFramework\myexcelproject\OR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B605EF7D-D274-446E-B9BB-83D60CE021DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{508BCCA8-023E-413A-ACDC-B890F26F1D57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
     <sheet name="LoginPage" sheetId="2" r:id="rId2"/>
-    <sheet name="Bank Manager Login" sheetId="3" r:id="rId3"/>
-    <sheet name="AddCustomer" sheetId="4" r:id="rId4"/>
-    <sheet name="OpenAccount" sheetId="5" r:id="rId5"/>
+    <sheet name="BankManagerLogin" sheetId="3" r:id="rId3"/>
+    <sheet name="DeleteCustomer" sheetId="6" r:id="rId4"/>
+    <sheet name="AddCustomer" sheetId="4" r:id="rId5"/>
+    <sheet name="OpenAccount" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
   <si>
     <t>Object</t>
   </si>
@@ -126,6 +127,15 @@
   </si>
   <si>
     <t>//select[@id='userSelect']</t>
+  </si>
+  <si>
+    <t>txtSearchCustomer</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Search Customer']</t>
+  </si>
+  <si>
+    <t>TextBox</t>
   </si>
 </sst>
 </file>
@@ -644,7 +654,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,6 +747,57 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF177766-BD50-4861-9E5A-1B24186DBD85}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="36.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Duplicate Value" error="An object already exists with this name." sqref="A1" xr:uid="{D90AD2D9-C06E-46BB-B92A-90E962FEE248}">
+      <formula1>COUNTIF($A$1:$A$999,A1)=1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -832,12 +893,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Major Version Update 25-02-2019
</commit_message>
<xml_diff>
--- a/myexcelproject/OR/ObjectRepository.xlsx
+++ b/myexcelproject/OR/ObjectRepository.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishna.teja.taduri\git\ExcelTestFramework\myexcelproject\OR\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{508BCCA8-023E-413A-ACDC-B890F26F1D57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B22FEBA8-B01F-42B6-93ED-8FD11D84F431}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14050" windowHeight="2410" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -21,6 +16,7 @@
     <sheet name="OpenAccount" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A2:K7"/>
 </workbook>
 </file>
 
@@ -142,16 +138,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -185,11 +173,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,7 +518,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,7 +641,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -686,7 +673,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
@@ -700,7 +687,7 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
@@ -714,7 +701,7 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
@@ -750,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF177766-BD50-4861-9E5A-1B24186DBD85}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -897,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>